<commit_message>
excel iterations with recruiter name
</commit_message>
<xml_diff>
--- a/Candidate_sheet.xlsx
+++ b/Candidate_sheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>First Name</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Postion</t>
+  </si>
+  <si>
+    <t>City</t>
   </si>
   <si>
     <t>Abhishek</t>
@@ -144,104 +147,122 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>8.213323121E9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>8.432134221E9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1">
         <v>9.432331424E9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1">
         <v>7.485232322E9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1">
         <v>9.423253224E9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>